<commit_message>
GBDS NOVEMBER 2025 FILES | UPDATED FILES
</commit_message>
<xml_diff>
--- a/GBDS NOVEMBER FILES 2025/CSR MONTH OF NOVEMBER.xlsx
+++ b/GBDS NOVEMBER FILES 2025/CSR MONTH OF NOVEMBER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GBDS NOVEMBER FILES 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDC7C35-8D8C-4CFC-B048-72862E7B02EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9E790A-3BA3-4924-80FC-E8F1A245CB7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{67C3A74A-A57E-4AB5-8CD3-31B592A14032}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{67C3A74A-A57E-4AB5-8CD3-31B592A14032}"/>
   </bookViews>
   <sheets>
     <sheet name="CSR | NOVEMBER" sheetId="902" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="11-03 R2" sheetId="1014" r:id="rId4"/>
     <sheet name="11-03 R3" sheetId="1015" r:id="rId5"/>
     <sheet name="(4)" sheetId="1016" r:id="rId6"/>
-    <sheet name="11-04 R1" sheetId="1017" r:id="rId7"/>
-    <sheet name="11-04 R2" sheetId="1018" r:id="rId8"/>
-    <sheet name="11-04 R3" sheetId="1019" r:id="rId9"/>
+    <sheet name="11-04 R2" sheetId="1018" r:id="rId7"/>
+    <sheet name="11-04 R3A" sheetId="1019" r:id="rId8"/>
+    <sheet name="11-04 R3B" sheetId="1017" r:id="rId9"/>
     <sheet name="(5)" sheetId="1020" r:id="rId10"/>
     <sheet name="11-05 R1" sheetId="1021" r:id="rId11"/>
     <sheet name="11-05 R2" sheetId="1022" r:id="rId12"/>
@@ -57,9 +57,9 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">'11-03 R1'!$A$1:$V$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'11-03 R2'!$A$1:$V$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'11-03 R3'!$A$1:$V$44</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">'11-04 R1'!$A$1:$V$44</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">'11-04 R2'!$A$1:$V$44</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="8">'11-04 R3'!$A$1:$V$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">'11-04 R2'!$A$1:$V$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">'11-04 R3A'!$A$1:$V$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">'11-04 R3B'!$A$1:$V$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="10">'11-05 R1'!$A$1:$V$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="11">'11-05 R2'!$A$1:$V$44</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="12">'11-05 R3'!$A$1:$V$44</definedName>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2365" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2377" uniqueCount="92">
   <si>
     <t>CHECKER STOCK REPORT</t>
   </si>
@@ -341,6 +341,33 @@
   </si>
   <si>
     <t>5/13B</t>
+  </si>
+  <si>
+    <t>ROUTE 3B</t>
+  </si>
+  <si>
+    <t>14/22B</t>
+  </si>
+  <si>
+    <t>6/23B</t>
+  </si>
+  <si>
+    <t>7/23B</t>
+  </si>
+  <si>
+    <t>15/1B</t>
+  </si>
+  <si>
+    <t>ROUTE 3A</t>
+  </si>
+  <si>
+    <t>36/1B</t>
+  </si>
+  <si>
+    <t>21B</t>
+  </si>
+  <si>
+    <t>35/4B</t>
   </si>
 </sst>
 </file>
@@ -1988,61 +2015,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>190502</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>22592</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>99392</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>215968</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF0CF60E-A336-4CD0-A204-EA32A7D0716A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8115302" y="5737592"/>
-          <a:ext cx="2147265" cy="1564976"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>77392</xdr:colOff>
       <xdr:row>35</xdr:row>
@@ -2094,7 +2066,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2138,6 +2110,61 @@
         <a:xfrm rot="10800000">
           <a:off x="7948612" y="6315305"/>
           <a:ext cx="2088357" cy="749860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>190502</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>22592</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>99392</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>215968</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF0CF60E-A336-4CD0-A204-EA32A7D0716A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8115302" y="5737592"/>
+          <a:ext cx="2147265" cy="1564976"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -37146,7 +37173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FBFA11-EE13-4CD3-BE99-8F548C5F47AD}">
   <dimension ref="B1:AA43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -40226,10 +40253,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A570865-4924-4A36-8B6D-652420F9B7E6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{111D1172-2E50-4DF4-BAEE-EDB58935E680}">
   <dimension ref="B1:AA43"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -40518,7 +40545,7 @@
     </row>
     <row r="7" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>38</v>
@@ -40583,12 +40610,18 @@
     </row>
     <row r="8" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="14">
+        <v>1</v>
+      </c>
+      <c r="D8" s="15">
+        <v>1</v>
+      </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>87</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -40598,11 +40631,17 @@
       <c r="O8" s="15"/>
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
+      <c r="R8" s="15">
+        <v>1</v>
+      </c>
       <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
+      <c r="T8" s="15">
+        <v>1</v>
+      </c>
       <c r="U8" s="62"/>
-      <c r="V8" s="16"/>
+      <c r="V8" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -40750,12 +40789,18 @@
       <c r="B15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
+      <c r="C15" s="23">
+        <v>1</v>
+      </c>
+      <c r="D15" s="24">
+        <v>1</v>
+      </c>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="24">
+        <v>0</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
@@ -40765,22 +40810,34 @@
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>
       <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
+      <c r="R15" s="24">
+        <v>1</v>
+      </c>
       <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
+      <c r="T15" s="24">
+        <v>1</v>
+      </c>
       <c r="U15" s="64"/>
-      <c r="V15" s="25"/>
+      <c r="V15" s="25">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
+      <c r="C16" s="60">
+        <v>0</v>
+      </c>
+      <c r="D16" s="61">
+        <v>0</v>
+      </c>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="67"/>
+      <c r="H16" s="29" t="s">
+        <v>87</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
@@ -40790,11 +40847,17 @@
       <c r="O16" s="29"/>
       <c r="P16" s="29"/>
       <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
+      <c r="R16" s="29">
+        <v>0</v>
+      </c>
       <c r="S16" s="29"/>
-      <c r="T16" s="59"/>
+      <c r="T16" s="59">
+        <v>0</v>
+      </c>
       <c r="U16" s="65"/>
-      <c r="V16" s="30"/>
+      <c r="V16" s="30">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="2:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
@@ -41177,16 +41240,28 @@
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="15">
+        <v>3</v>
+      </c>
       <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
+      <c r="J24" s="15">
+        <v>67</v>
+      </c>
       <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="L24" s="15">
+        <v>3</v>
+      </c>
+      <c r="M24" s="15">
+        <v>15</v>
+      </c>
+      <c r="N24" s="15">
+        <v>356</v>
+      </c>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
+      <c r="Q24" s="15">
+        <v>5</v>
+      </c>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
@@ -41342,16 +41417,28 @@
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="24">
+        <v>3</v>
+      </c>
       <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="J31" s="24">
+        <v>17</v>
+      </c>
       <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
+      <c r="L31" s="24">
+        <v>3</v>
+      </c>
+      <c r="M31" s="24">
+        <v>5</v>
+      </c>
+      <c r="N31" s="24">
+        <v>14</v>
+      </c>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="Q31" s="24">
+        <v>5</v>
+      </c>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
@@ -41367,16 +41454,28 @@
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29">
+        <v>0</v>
+      </c>
       <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
+      <c r="J32" s="29">
+        <v>50</v>
+      </c>
       <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="L32" s="29">
+        <v>0</v>
+      </c>
+      <c r="M32" s="29">
+        <v>10</v>
+      </c>
+      <c r="N32" s="29">
+        <v>342</v>
+      </c>
       <c r="O32" s="24"/>
       <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="29">
+        <v>0</v>
+      </c>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -41505,8 +41604,12 @@
       <c r="C36" s="49"/>
       <c r="D36" s="44"/>
       <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
+      <c r="F36" s="45">
+        <v>412</v>
+      </c>
+      <c r="G36" s="45">
+        <v>25</v>
+      </c>
       <c r="H36" s="45"/>
       <c r="I36" s="45"/>
       <c r="J36" s="45"/>
@@ -41514,8 +41617,12 @@
       <c r="L36" s="45"/>
       <c r="M36" s="45"/>
       <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
+      <c r="O36" s="45">
+        <v>5</v>
+      </c>
+      <c r="P36" s="45">
+        <v>31</v>
+      </c>
       <c r="Q36" s="46"/>
       <c r="R36" s="40"/>
       <c r="S36" s="40"/>
@@ -41645,8 +41752,12 @@
       <c r="C42" s="49"/>
       <c r="D42" s="44"/>
       <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
+      <c r="F42" s="45">
+        <v>412</v>
+      </c>
+      <c r="G42" s="45">
+        <v>25</v>
+      </c>
       <c r="H42" s="45"/>
       <c r="I42" s="45"/>
       <c r="J42" s="45"/>
@@ -41654,8 +41765,12 @@
       <c r="L42" s="45"/>
       <c r="M42" s="45"/>
       <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
+      <c r="O42" s="45">
+        <v>5</v>
+      </c>
+      <c r="P42" s="45">
+        <v>31</v>
+      </c>
       <c r="Q42" s="46"/>
       <c r="R42" s="71" t="s">
         <v>54</v>
@@ -41707,7 +41822,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{111D1172-2E50-4DF4-BAEE-EDB58935E680}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3E96A2-155A-4362-9251-0996248BEECE}">
   <dimension ref="B1:AA43"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
@@ -41999,7 +42114,7 @@
     </row>
     <row r="7" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>38</v>
@@ -42064,12 +42179,18 @@
     </row>
     <row r="8" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="14">
+        <v>1</v>
+      </c>
+      <c r="D8" s="15">
+        <v>1</v>
+      </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>89</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -42079,11 +42200,17 @@
       <c r="O8" s="15"/>
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
+      <c r="R8" s="15">
+        <v>2</v>
+      </c>
       <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
+      <c r="T8" s="15">
+        <v>3</v>
+      </c>
       <c r="U8" s="62"/>
-      <c r="V8" s="16"/>
+      <c r="V8" s="16">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -42231,12 +42358,18 @@
       <c r="B15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
+      <c r="C15" s="23">
+        <v>1</v>
+      </c>
+      <c r="D15" s="24">
+        <v>1</v>
+      </c>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>90</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
@@ -42246,22 +42379,34 @@
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>
       <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
+      <c r="R15" s="24">
+        <v>2</v>
+      </c>
       <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
+      <c r="T15" s="24">
+        <v>0</v>
+      </c>
       <c r="U15" s="64"/>
-      <c r="V15" s="25"/>
+      <c r="V15" s="25">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
+      <c r="C16" s="60">
+        <v>0</v>
+      </c>
+      <c r="D16" s="61">
+        <v>0</v>
+      </c>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
+      <c r="H16" s="29" t="s">
+        <v>91</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
@@ -42271,11 +42416,17 @@
       <c r="O16" s="29"/>
       <c r="P16" s="29"/>
       <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
+      <c r="R16" s="29">
+        <v>0</v>
+      </c>
       <c r="S16" s="29"/>
-      <c r="T16" s="59"/>
+      <c r="T16" s="59">
+        <v>3</v>
+      </c>
       <c r="U16" s="65"/>
-      <c r="V16" s="30"/>
+      <c r="V16" s="30">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="2:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
@@ -42653,21 +42804,35 @@
       <c r="B24" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="14"/>
+      <c r="C24" s="14">
+        <v>1</v>
+      </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="15">
+        <v>2</v>
+      </c>
       <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
+      <c r="J24" s="15">
+        <v>147</v>
+      </c>
       <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="L24" s="15">
+        <v>2</v>
+      </c>
+      <c r="M24" s="15">
+        <v>16</v>
+      </c>
+      <c r="N24" s="15">
+        <v>757</v>
+      </c>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
+      <c r="Q24" s="15">
+        <v>3</v>
+      </c>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
@@ -42818,21 +42983,35 @@
       <c r="B31" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="23"/>
+      <c r="C31" s="23">
+        <v>0</v>
+      </c>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="24">
+        <v>0</v>
+      </c>
       <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="J31" s="24">
+        <v>0</v>
+      </c>
       <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
+      <c r="L31" s="24">
+        <v>0</v>
+      </c>
+      <c r="M31" s="24">
+        <v>0</v>
+      </c>
+      <c r="N31" s="24">
+        <v>54</v>
+      </c>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="Q31" s="24">
+        <v>3</v>
+      </c>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
@@ -42843,21 +43022,35 @@
       <c r="B32" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="27"/>
+      <c r="C32" s="27">
+        <v>1</v>
+      </c>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29">
+        <v>2</v>
+      </c>
       <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
+      <c r="J32" s="29">
+        <v>147</v>
+      </c>
       <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="L32" s="29">
+        <v>2</v>
+      </c>
+      <c r="M32" s="29">
+        <v>16</v>
+      </c>
+      <c r="N32" s="29">
+        <v>703</v>
+      </c>
       <c r="O32" s="24"/>
       <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="29">
+        <v>0</v>
+      </c>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -42983,20 +43176,44 @@
       <c r="B36" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="49"/>
+      <c r="C36" s="49">
+        <v>2</v>
+      </c>
       <c r="D36" s="44"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
+      <c r="E36" s="45">
+        <v>18</v>
+      </c>
+      <c r="F36" s="45">
+        <v>959</v>
+      </c>
+      <c r="G36" s="45">
+        <v>4</v>
+      </c>
       <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
+      <c r="I36" s="45">
+        <v>19</v>
+      </c>
+      <c r="J36" s="45">
+        <v>1</v>
+      </c>
+      <c r="K36" s="45">
+        <v>8</v>
+      </c>
+      <c r="L36" s="45">
+        <v>6</v>
+      </c>
+      <c r="M36" s="45">
+        <v>2</v>
+      </c>
+      <c r="N36" s="45">
+        <v>5</v>
+      </c>
+      <c r="O36" s="45">
+        <v>20</v>
+      </c>
+      <c r="P36" s="45">
+        <v>8</v>
+      </c>
       <c r="Q36" s="46"/>
       <c r="R36" s="40"/>
       <c r="S36" s="40"/>
@@ -43123,20 +43340,44 @@
       <c r="B42" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="49"/>
+      <c r="C42" s="49">
+        <v>2</v>
+      </c>
       <c r="D42" s="44"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
+      <c r="E42" s="45">
+        <v>18</v>
+      </c>
+      <c r="F42" s="45">
+        <v>959</v>
+      </c>
+      <c r="G42" s="45">
+        <v>4</v>
+      </c>
       <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
+      <c r="I42" s="45">
+        <v>19</v>
+      </c>
+      <c r="J42" s="45">
+        <v>1</v>
+      </c>
+      <c r="K42" s="45">
+        <v>8</v>
+      </c>
+      <c r="L42" s="45">
+        <v>6</v>
+      </c>
+      <c r="M42" s="45">
+        <v>2</v>
+      </c>
+      <c r="N42" s="45">
+        <v>5</v>
+      </c>
+      <c r="O42" s="45">
+        <v>20</v>
+      </c>
+      <c r="P42" s="45">
+        <v>8</v>
+      </c>
       <c r="Q42" s="46"/>
       <c r="R42" s="71" t="s">
         <v>54</v>
@@ -43188,11 +43429,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3E96A2-155A-4362-9251-0996248BEECE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A570865-4924-4A36-8B6D-652420F9B7E6}">
   <dimension ref="B1:AA43"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F36" sqref="F36:Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -43480,7 +43721,7 @@
     </row>
     <row r="7" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>38</v>
@@ -43545,12 +43786,18 @@
     </row>
     <row r="8" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="15">
+        <v>1</v>
+      </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>84</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
@@ -43562,9 +43809,13 @@
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
       <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
+      <c r="T8" s="15">
+        <v>1</v>
+      </c>
       <c r="U8" s="62"/>
-      <c r="V8" s="16"/>
+      <c r="V8" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="2:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -43712,12 +43963,18 @@
       <c r="B15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
+      <c r="C15" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="24">
+        <v>1</v>
+      </c>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>85</v>
+      </c>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
@@ -43729,20 +43986,30 @@
       <c r="Q15" s="24"/>
       <c r="R15" s="24"/>
       <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
+      <c r="T15" s="24">
+        <v>1</v>
+      </c>
       <c r="U15" s="64"/>
-      <c r="V15" s="25"/>
+      <c r="V15" s="25">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="2:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
+      <c r="C16" s="60">
+        <v>0</v>
+      </c>
+      <c r="D16" s="61">
+        <v>0</v>
+      </c>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
+      <c r="H16" s="67" t="s">
+        <v>86</v>
+      </c>
       <c r="I16" s="29"/>
       <c r="J16" s="29"/>
       <c r="K16" s="59"/>
@@ -43754,9 +44021,13 @@
       <c r="Q16" s="29"/>
       <c r="R16" s="29"/>
       <c r="S16" s="29"/>
-      <c r="T16" s="59"/>
+      <c r="T16" s="59">
+        <v>0</v>
+      </c>
       <c r="U16" s="65"/>
-      <c r="V16" s="30"/>
+      <c r="V16" s="30">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="2:22" s="5" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
@@ -44139,16 +44410,28 @@
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="15" t="s">
+        <v>73</v>
+      </c>
       <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
+      <c r="J24" s="15">
+        <v>30</v>
+      </c>
       <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
+      <c r="L24" s="15">
+        <v>1</v>
+      </c>
+      <c r="M24" s="15">
+        <v>5</v>
+      </c>
+      <c r="N24" s="15">
+        <v>298</v>
+      </c>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
+      <c r="Q24" s="15">
+        <v>9</v>
+      </c>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
@@ -44304,16 +44587,28 @@
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="24" t="s">
+        <v>73</v>
+      </c>
       <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
+      <c r="J31" s="24">
+        <v>20</v>
+      </c>
       <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
+      <c r="L31" s="24">
+        <v>1</v>
+      </c>
+      <c r="M31" s="24">
+        <v>1</v>
+      </c>
+      <c r="N31" s="24">
+        <v>85</v>
+      </c>
       <c r="O31" s="24"/>
       <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
+      <c r="Q31" s="24">
+        <v>9</v>
+      </c>
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
       <c r="T31" s="24"/>
@@ -44329,16 +44624,28 @@
       <c r="E32" s="28"/>
       <c r="F32" s="28"/>
       <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="H32" s="29">
+        <v>0</v>
+      </c>
       <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
+      <c r="J32" s="29">
+        <v>10</v>
+      </c>
       <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="L32" s="29">
+        <v>0</v>
+      </c>
+      <c r="M32" s="29">
+        <v>4</v>
+      </c>
+      <c r="N32" s="29">
+        <v>213</v>
+      </c>
       <c r="O32" s="24"/>
       <c r="P32" s="29"/>
-      <c r="Q32" s="29"/>
+      <c r="Q32" s="29">
+        <v>0</v>
+      </c>
       <c r="R32" s="29"/>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -44467,18 +44774,36 @@
       <c r="C36" s="49"/>
       <c r="D36" s="44"/>
       <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
+      <c r="F36" s="45">
+        <v>285</v>
+      </c>
       <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
+      <c r="H36" s="45">
+        <v>2</v>
+      </c>
+      <c r="I36" s="45">
+        <v>6</v>
+      </c>
+      <c r="J36" s="45">
+        <v>1</v>
+      </c>
+      <c r="K36" s="45">
+        <v>7</v>
+      </c>
       <c r="L36" s="45"/>
       <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="46"/>
+      <c r="N36" s="45">
+        <v>25</v>
+      </c>
+      <c r="O36" s="45">
+        <v>3</v>
+      </c>
+      <c r="P36" s="45">
+        <v>3</v>
+      </c>
+      <c r="Q36" s="46">
+        <v>20</v>
+      </c>
       <c r="R36" s="40"/>
       <c r="S36" s="40"/>
       <c r="T36" s="40"/>
@@ -44607,18 +44932,36 @@
       <c r="C42" s="49"/>
       <c r="D42" s="44"/>
       <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
+      <c r="F42" s="45">
+        <v>285</v>
+      </c>
       <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
+      <c r="H42" s="45">
+        <v>2</v>
+      </c>
+      <c r="I42" s="45">
+        <v>6</v>
+      </c>
+      <c r="J42" s="45">
+        <v>1</v>
+      </c>
+      <c r="K42" s="45">
+        <v>7</v>
+      </c>
       <c r="L42" s="45"/>
       <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="46"/>
+      <c r="N42" s="45">
+        <v>25</v>
+      </c>
+      <c r="O42" s="45">
+        <v>3</v>
+      </c>
+      <c r="P42" s="45">
+        <v>3</v>
+      </c>
+      <c r="Q42" s="46">
+        <v>20</v>
+      </c>
       <c r="R42" s="71" t="s">
         <v>54</v>
       </c>

</xml_diff>